<commit_message>
add lookup table data to excel file
</commit_message>
<xml_diff>
--- a/TabeebkServer/src/main/webapp/bulkUpload/downloadexcelFile/MspData.xlsx
+++ b/TabeebkServer/src/main/webapp/bulkUpload/downloadexcelFile/MspData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="510" windowWidth="14055" windowHeight="6345" activeTab="11"/>
+    <workbookView xWindow="510" yWindow="510" windowWidth="14055" windowHeight="6345" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Doctor" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
   <si>
     <t>DoctorNameEn</t>
   </si>
@@ -103,9 +103,6 @@
     <t>LabHosbital</t>
   </si>
   <si>
-    <t>cairo</t>
-  </si>
-  <si>
     <t>ClinicTel</t>
   </si>
   <si>
@@ -118,12 +115,6 @@
     <t>labTel</t>
   </si>
   <si>
-    <t>ismailia</t>
-  </si>
-  <si>
-    <t>suez</t>
-  </si>
-  <si>
     <t>ClincImage</t>
   </si>
   <si>
@@ -133,12 +124,6 @@
     <t>fullAddressAr</t>
   </si>
   <si>
-    <t>Dentist</t>
-  </si>
-  <si>
-    <t>Midwife</t>
-  </si>
-  <si>
     <t>SpecialityName</t>
   </si>
   <si>
@@ -148,19 +133,130 @@
     <t>DoctorTel</t>
   </si>
   <si>
-    <t>banha</t>
-  </si>
-  <si>
-    <t>Microbiology</t>
-  </si>
-  <si>
-    <t>Parasitology</t>
-  </si>
-  <si>
     <t>ClincNameEn</t>
   </si>
   <si>
     <t>ClincNameAr</t>
+  </si>
+  <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Giza</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Luxor</t>
+  </si>
+  <si>
+    <t>Behira</t>
+  </si>
+  <si>
+    <t>Aswan</t>
+  </si>
+  <si>
+    <t>Bani Suef</t>
+  </si>
+  <si>
+    <t>Dakahlia</t>
+  </si>
+  <si>
+    <t>Damiatta</t>
+  </si>
+  <si>
+    <t>Fayoum</t>
+  </si>
+  <si>
+    <t>Gharbeya</t>
+  </si>
+  <si>
+    <t>Red Sea</t>
+  </si>
+  <si>
+    <t>Ismailia</t>
+  </si>
+  <si>
+    <t>Kafr El Sheikh</t>
+  </si>
+  <si>
+    <t>Marsa Matrouh</t>
+  </si>
+  <si>
+    <t>Menia</t>
+  </si>
+  <si>
+    <t>Menophia</t>
+  </si>
+  <si>
+    <t>Port Said</t>
+  </si>
+  <si>
+    <t>Qalioubia</t>
+  </si>
+  <si>
+    <t>Quena</t>
+  </si>
+  <si>
+    <t>Sharqeya</t>
+  </si>
+  <si>
+    <t>Sohag</t>
+  </si>
+  <si>
+    <t>Suez</t>
+  </si>
+  <si>
+    <t>Assuit</t>
+  </si>
+  <si>
+    <t>Sinai</t>
+  </si>
+  <si>
+    <t>Banha</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Cardiovascular</t>
+  </si>
+  <si>
+    <t>Orthopedics</t>
+  </si>
+  <si>
+    <t>Obstetrics &amp; Gynaecology</t>
+  </si>
+  <si>
+    <t>Neurology</t>
+  </si>
+  <si>
+    <t>Pulmonary</t>
+  </si>
+  <si>
+    <t>Endocrinology</t>
+  </si>
+  <si>
+    <t>Paediatrics</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t>Ophthalmology   </t>
+  </si>
+  <si>
+    <t>Otorhinology</t>
+  </si>
+  <si>
+    <t>Radiology Center</t>
+  </si>
+  <si>
+    <t>Physiotherapy</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
   </si>
 </sst>
 </file>
@@ -213,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -222,7 +318,8 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -569,7 +666,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -713,7 +810,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -746,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -772,10 +869,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -936,7 +1033,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -972,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1048,10 +1145,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1088,90 +1185,287 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A2">
-      <formula1>$I$1:$I$2</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>40</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1198,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1247,16 +1541,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1310,10 +1604,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1351,7 +1645,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1364,7 +1658,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1376,10 +1670,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1623,10 +1917,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>